<commit_message>
Added more data points to uranium.xlsx, datetime info pending
</commit_message>
<xml_diff>
--- a/uranium.xlsx
+++ b/uranium.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ikansh\CS\uranium-soil-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7F9F7D-9CEB-4BC7-8D73-431D7D736D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA730C9E-E9E8-4FB0-82B7-A323A9F1A70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="High U-contents observed in som" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Uranium Content Anomalies in Gr" sheetId="2" r:id="rId2"/>
+    <sheet name="Comparative statistical analysi" sheetId="3" r:id="rId3"/>
+    <sheet name="Uranium studies in water sample" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="199">
   <si>
     <t>Location</t>
   </si>
@@ -197,6 +199,432 @@
   </si>
   <si>
     <t>Sohan Garh urf Ratte</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/338209223_Uranium_Content_Anomalies_in_Groundwaters_of_Ferozepur_District_of_Punjab_India_and_the_Corresponding_Risk_Factors/</t>
+  </si>
+  <si>
+    <t>District (no. of samples)</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>P 5</t>
+  </si>
+  <si>
+    <t>P 25</t>
+  </si>
+  <si>
+    <t>P 75</t>
+  </si>
+  <si>
+    <t>P 95</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Mansa (47)</t>
+  </si>
+  <si>
+    <t>Uranium concentration</t>
+  </si>
+  <si>
+    <t>Excess Cancer risk</t>
+  </si>
+  <si>
+    <t>2.70×10 −4</t>
+  </si>
+  <si>
+    <t>1.43×10 −4</t>
+  </si>
+  <si>
+    <t>2.41×10 −5</t>
+  </si>
+  <si>
+    <t>7.02×10 −5</t>
+  </si>
+  <si>
+    <t>2.72×10 −4</t>
+  </si>
+  <si>
+    <t>9.12×10 −4</t>
+  </si>
+  <si>
+    <t>1.6×10 −5</t>
+  </si>
+  <si>
+    <t>1.80×10 −3</t>
+  </si>
+  <si>
+    <t>LADD</t>
+  </si>
+  <si>
+    <t>HQ</t>
+  </si>
+  <si>
+    <t>Bathinda (46)</t>
+  </si>
+  <si>
+    <t>1.94×10 −4</t>
+  </si>
+  <si>
+    <t>1.04×10 −4</t>
+  </si>
+  <si>
+    <t>2.33×10 −5</t>
+  </si>
+  <si>
+    <t>5.88×10 −5</t>
+  </si>
+  <si>
+    <t>2.35×10 −4</t>
+  </si>
+  <si>
+    <t>6.18×10 −4</t>
+  </si>
+  <si>
+    <t>2.21×10 −5</t>
+  </si>
+  <si>
+    <t>9.07×10 −4</t>
+  </si>
+  <si>
+    <t>Faridkot (48)</t>
+  </si>
+  <si>
+    <t>2.45×10 −4</t>
+  </si>
+  <si>
+    <t>1.48×10 −4</t>
+  </si>
+  <si>
+    <t>2.22×10 −5</t>
+  </si>
+  <si>
+    <t>7.41×10 −5</t>
+  </si>
+  <si>
+    <t>2.61×10 −4</t>
+  </si>
+  <si>
+    <t>8.4×10 −4</t>
+  </si>
+  <si>
+    <t>2.13×10 −5</t>
+  </si>
+  <si>
+    <t>1.05×10 −4</t>
+  </si>
+  <si>
+    <t>Tarn-taran (38)</t>
+  </si>
+  <si>
+    <t>1.03×10 −4</t>
+  </si>
+  <si>
+    <t>6.98×10 −5</t>
+  </si>
+  <si>
+    <t>9.52×10 −6</t>
+  </si>
+  <si>
+    <t>2.76×10 −5</t>
+  </si>
+  <si>
+    <t>1.10×10 −4</t>
+  </si>
+  <si>
+    <t>2.62×10 −4</t>
+  </si>
+  <si>
+    <t>7.33×10 −6</t>
+  </si>
+  <si>
+    <t>3.81×10 −4</t>
+  </si>
+  <si>
+    <t>Amritsar (39)</t>
+  </si>
+  <si>
+    <t>3.12×10 −5</t>
+  </si>
+  <si>
+    <t>2.02×10 −5</t>
+  </si>
+  <si>
+    <t>3.27×10 −6</t>
+  </si>
+  <si>
+    <t>9.40×10 −6</t>
+  </si>
+  <si>
+    <t>3.74×10 −5</t>
+  </si>
+  <si>
+    <t>9.67×10 −5</t>
+  </si>
+  <si>
+    <t>2.43×10 −6</t>
+  </si>
+  <si>
+    <t>1.19×10 −4</t>
+  </si>
+  <si>
+    <t>Hoshiarpur (48)</t>
+  </si>
+  <si>
+    <t>1.32×10 −5</t>
+  </si>
+  <si>
+    <t>8.23×10 −6</t>
+  </si>
+  <si>
+    <t>1.54×10 −6</t>
+  </si>
+  <si>
+    <t>3.47×10 −6</t>
+  </si>
+  <si>
+    <t>1.64×10 −5</t>
+  </si>
+  <si>
+    <t>3.85×10 −5</t>
+  </si>
+  <si>
+    <t>1.34×10 −6</t>
+  </si>
+  <si>
+    <t>7.05×10 −5</t>
+  </si>
+  <si>
+    <t>Uranium concentration (μg/l)</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0969804316307035</t>
+  </si>
+  <si>
+    <t>Sr. No.</t>
+  </si>
+  <si>
+    <t>Sample location (Village)</t>
+  </si>
+  <si>
+    <t>Sangrur</t>
+  </si>
+  <si>
+    <t>Tapa</t>
+  </si>
+  <si>
+    <t>12.93±0.15 a</t>
+  </si>
+  <si>
+    <t>Handiaya</t>
+  </si>
+  <si>
+    <t>14.42±0.16</t>
+  </si>
+  <si>
+    <t>Barnala</t>
+  </si>
+  <si>
+    <t>5.41±0.10</t>
+  </si>
+  <si>
+    <t>9.37±0.13</t>
+  </si>
+  <si>
+    <t>Bhawanigarh</t>
+  </si>
+  <si>
+    <t>13.42±0.16</t>
+  </si>
+  <si>
+    <t>Dhuri</t>
+  </si>
+  <si>
+    <t>19.43±0.19</t>
+  </si>
+  <si>
+    <t>Dhanola</t>
+  </si>
+  <si>
+    <t>21.24±0.20</t>
+  </si>
+  <si>
+    <t>Sunam</t>
+  </si>
+  <si>
+    <t>20.13±0.20</t>
+  </si>
+  <si>
+    <t>Malerkotla</t>
+  </si>
+  <si>
+    <t>8.43±0.12</t>
+  </si>
+  <si>
+    <t>Faridkot</t>
+  </si>
+  <si>
+    <t>10.43±0.14</t>
+  </si>
+  <si>
+    <t>Sadik</t>
+  </si>
+  <si>
+    <t>13.95±0.16</t>
+  </si>
+  <si>
+    <t>Kot Kapura</t>
+  </si>
+  <si>
+    <t>17.88±0.18</t>
+  </si>
+  <si>
+    <t>Khara</t>
+  </si>
+  <si>
+    <t>16.32±0.13</t>
+  </si>
+  <si>
+    <t>Jaiton</t>
+  </si>
+  <si>
+    <t>19.32±0.19</t>
+  </si>
+  <si>
+    <t>Mansa</t>
+  </si>
+  <si>
+    <t>Budlada</t>
+  </si>
+  <si>
+    <t>11.78±0.15</t>
+  </si>
+  <si>
+    <t>26.93±0.24</t>
+  </si>
+  <si>
+    <t>Burj Harike</t>
+  </si>
+  <si>
+    <t>43.39±0.29</t>
+  </si>
+  <si>
+    <t>Bhiki</t>
+  </si>
+  <si>
+    <t>14.33±0.16</t>
+  </si>
+  <si>
+    <t>Bareta</t>
+  </si>
+  <si>
+    <t>16.68±0.17</t>
+  </si>
+  <si>
+    <t>Patiala</t>
+  </si>
+  <si>
+    <t>Nabha</t>
+  </si>
+  <si>
+    <t>20.21±0.20</t>
+  </si>
+  <si>
+    <t>21.43±0.20</t>
+  </si>
+  <si>
+    <t>Samana</t>
+  </si>
+  <si>
+    <t>14.43±0.16</t>
+  </si>
+  <si>
+    <t>Kauli</t>
+  </si>
+  <si>
+    <t>30.41±0.24</t>
+  </si>
+  <si>
+    <t>Raj Pura</t>
+  </si>
+  <si>
+    <t>10.73±0.14</t>
+  </si>
+  <si>
+    <t>Ludhiana</t>
+  </si>
+  <si>
+    <t>RaiKot</t>
+  </si>
+  <si>
+    <t>11.68±0.15</t>
+  </si>
+  <si>
+    <t>27.35±0.23</t>
+  </si>
+  <si>
+    <t>Khanna</t>
+  </si>
+  <si>
+    <t>6.78±0.14</t>
+  </si>
+  <si>
+    <t>Sarhind</t>
+  </si>
+  <si>
+    <t>30.31±0.24</t>
+  </si>
+  <si>
+    <t>Jagraon</t>
+  </si>
+  <si>
+    <t>20.43±0.20</t>
+  </si>
+  <si>
+    <t>Moga</t>
+  </si>
+  <si>
+    <t>19.42±0.20</t>
+  </si>
+  <si>
+    <t>Baga Purana</t>
+  </si>
+  <si>
+    <t>17.43±0.17</t>
+  </si>
+  <si>
+    <t>Smalsar</t>
+  </si>
+  <si>
+    <t>9.45±0.13</t>
+  </si>
+  <si>
+    <t>Ajitwal</t>
+  </si>
+  <si>
+    <t>5.50±0.10</t>
+  </si>
+  <si>
+    <t>Nihal Singh Wala</t>
+  </si>
+  <si>
+    <t>17.80±0.18</t>
+  </si>
+  <si>
+    <t>Uranium concentration in water (μg/l)</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S1350448707000492</t>
   </si>
 </sst>
 </file>
@@ -253,13 +681,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -543,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -558,19 +987,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -844,15 +1273,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F64A2C-8E6C-4CCC-8F64-2489DDB0ACAF}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="1" max="1" width="32.21875" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.5546875" style="2" customWidth="1"/>
@@ -1574,7 +2003,1273 @@
         <v>1.31</v>
       </c>
     </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A37" r:id="rId1" xr:uid="{59C2BA6D-A367-4FA3-8008-04D1FE42453D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB6283E-33DE-4F60-9242-7912B3442B6F}">
+  <dimension ref="A1:L30"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.21875" customWidth="1"/>
+    <col min="2" max="2" width="33.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" customWidth="1"/>
+    <col min="12" max="12" width="61.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2">
+        <v>96.46</v>
+      </c>
+      <c r="D2">
+        <v>51.11</v>
+      </c>
+      <c r="E2">
+        <v>8.64</v>
+      </c>
+      <c r="F2">
+        <v>25.1</v>
+      </c>
+      <c r="G2">
+        <v>97.22</v>
+      </c>
+      <c r="H2">
+        <v>325.95999999999998</v>
+      </c>
+      <c r="I2">
+        <v>5.9</v>
+      </c>
+      <c r="J2">
+        <v>645.22</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <v>7.27</v>
+      </c>
+      <c r="D4">
+        <v>3.85</v>
+      </c>
+      <c r="E4">
+        <v>0.65</v>
+      </c>
+      <c r="F4">
+        <v>1.89</v>
+      </c>
+      <c r="G4">
+        <v>7.33</v>
+      </c>
+      <c r="H4">
+        <v>24.57</v>
+      </c>
+      <c r="I4">
+        <v>0.44</v>
+      </c>
+      <c r="J4">
+        <v>48.65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5">
+        <v>1.6</v>
+      </c>
+      <c r="D5">
+        <v>0.85</v>
+      </c>
+      <c r="E5">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F5">
+        <v>0.42</v>
+      </c>
+      <c r="G5">
+        <v>1.61</v>
+      </c>
+      <c r="H5">
+        <v>5.42</v>
+      </c>
+      <c r="I5">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="J5">
+        <v>10.73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7">
+        <v>69.349999999999994</v>
+      </c>
+      <c r="D7">
+        <v>37.44</v>
+      </c>
+      <c r="E7">
+        <v>8.33</v>
+      </c>
+      <c r="F7">
+        <v>21.03</v>
+      </c>
+      <c r="G7">
+        <v>83.94</v>
+      </c>
+      <c r="H7">
+        <v>220.75</v>
+      </c>
+      <c r="I7">
+        <v>7.9</v>
+      </c>
+      <c r="J7">
+        <v>323.94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I8" t="s">
+        <v>87</v>
+      </c>
+      <c r="J8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9">
+        <v>5.23</v>
+      </c>
+      <c r="D9">
+        <v>2.82</v>
+      </c>
+      <c r="E9">
+        <v>0.63</v>
+      </c>
+      <c r="F9">
+        <v>1.58</v>
+      </c>
+      <c r="G9">
+        <v>6.33</v>
+      </c>
+      <c r="H9">
+        <v>16.64</v>
+      </c>
+      <c r="I9">
+        <v>0.59</v>
+      </c>
+      <c r="J9">
+        <v>24.42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D10">
+        <v>0.62</v>
+      </c>
+      <c r="E10">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F10">
+        <v>0.35</v>
+      </c>
+      <c r="G10">
+        <v>1.4</v>
+      </c>
+      <c r="H10">
+        <v>3.67</v>
+      </c>
+      <c r="I10">
+        <v>0.13</v>
+      </c>
+      <c r="J10">
+        <v>5.39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12">
+        <v>87.85</v>
+      </c>
+      <c r="D12">
+        <v>52.94</v>
+      </c>
+      <c r="E12">
+        <v>7.94</v>
+      </c>
+      <c r="F12">
+        <v>26.49</v>
+      </c>
+      <c r="G12">
+        <v>93.3</v>
+      </c>
+      <c r="H12">
+        <v>300.3</v>
+      </c>
+      <c r="I12">
+        <v>7.62</v>
+      </c>
+      <c r="J12">
+        <v>375.85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" t="s">
+        <v>94</v>
+      </c>
+      <c r="H13" t="s">
+        <v>95</v>
+      </c>
+      <c r="I13" t="s">
+        <v>96</v>
+      </c>
+      <c r="J13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14">
+        <v>6.62</v>
+      </c>
+      <c r="D14">
+        <v>3.99</v>
+      </c>
+      <c r="E14">
+        <v>0.6</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>7.03</v>
+      </c>
+      <c r="H14">
+        <v>22.64</v>
+      </c>
+      <c r="I14">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J14">
+        <v>22.64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15">
+        <v>1.46</v>
+      </c>
+      <c r="D15">
+        <v>0.88</v>
+      </c>
+      <c r="E15">
+        <v>0.13</v>
+      </c>
+      <c r="F15">
+        <v>0.44</v>
+      </c>
+      <c r="G15">
+        <v>1.55</v>
+      </c>
+      <c r="H15">
+        <v>4.99</v>
+      </c>
+      <c r="I15">
+        <v>0.12</v>
+      </c>
+      <c r="J15">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17">
+        <v>36.92</v>
+      </c>
+      <c r="D17">
+        <v>24.93</v>
+      </c>
+      <c r="E17">
+        <v>3.4</v>
+      </c>
+      <c r="F17">
+        <v>9.8699999999999992</v>
+      </c>
+      <c r="G17">
+        <v>39.31</v>
+      </c>
+      <c r="H17">
+        <v>93.78</v>
+      </c>
+      <c r="I17">
+        <v>2.62</v>
+      </c>
+      <c r="J17">
+        <v>136.13999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" t="s">
+        <v>102</v>
+      </c>
+      <c r="G18" t="s">
+        <v>103</v>
+      </c>
+      <c r="H18" t="s">
+        <v>104</v>
+      </c>
+      <c r="I18" t="s">
+        <v>105</v>
+      </c>
+      <c r="J18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19">
+        <v>2.78</v>
+      </c>
+      <c r="D19">
+        <v>1.88</v>
+      </c>
+      <c r="E19">
+        <v>0.26</v>
+      </c>
+      <c r="F19">
+        <v>0.74</v>
+      </c>
+      <c r="G19">
+        <v>2.96</v>
+      </c>
+      <c r="H19">
+        <v>7.07</v>
+      </c>
+      <c r="I19">
+        <v>0.2</v>
+      </c>
+      <c r="J19">
+        <v>10.26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20">
+        <v>0.61</v>
+      </c>
+      <c r="D20">
+        <v>0.41</v>
+      </c>
+      <c r="E20">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="F20">
+        <v>0.16</v>
+      </c>
+      <c r="G20">
+        <v>0.65</v>
+      </c>
+      <c r="H20">
+        <v>1.56</v>
+      </c>
+      <c r="I20">
+        <v>0.04</v>
+      </c>
+      <c r="J20">
+        <v>2.2599999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22">
+        <v>11.14</v>
+      </c>
+      <c r="D22">
+        <v>7.22</v>
+      </c>
+      <c r="E22">
+        <v>1.17</v>
+      </c>
+      <c r="F22">
+        <v>3.36</v>
+      </c>
+      <c r="G22">
+        <v>13.37</v>
+      </c>
+      <c r="H22">
+        <v>34.54</v>
+      </c>
+      <c r="I22">
+        <v>0.87</v>
+      </c>
+      <c r="J22">
+        <v>42.51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D23" t="s">
+        <v>109</v>
+      </c>
+      <c r="E23" t="s">
+        <v>110</v>
+      </c>
+      <c r="F23" t="s">
+        <v>111</v>
+      </c>
+      <c r="G23" t="s">
+        <v>112</v>
+      </c>
+      <c r="H23" t="s">
+        <v>113</v>
+      </c>
+      <c r="I23" t="s">
+        <v>114</v>
+      </c>
+      <c r="J23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24">
+        <v>0.84</v>
+      </c>
+      <c r="D24">
+        <v>0.54</v>
+      </c>
+      <c r="E24">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="F24">
+        <v>0.25</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>2.6</v>
+      </c>
+      <c r="I24">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="J24">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25">
+        <v>0.18</v>
+      </c>
+      <c r="D25">
+        <v>0.12</v>
+      </c>
+      <c r="E25">
+        <v>1.9E-2</v>
+      </c>
+      <c r="F25">
+        <v>5.5E-2</v>
+      </c>
+      <c r="G25">
+        <v>0.22</v>
+      </c>
+      <c r="H25">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="I25">
+        <v>1.4E-2</v>
+      </c>
+      <c r="J25">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27">
+        <v>4.74</v>
+      </c>
+      <c r="D27">
+        <v>2.94</v>
+      </c>
+      <c r="E27">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F27">
+        <v>1.24</v>
+      </c>
+      <c r="G27">
+        <v>5.88</v>
+      </c>
+      <c r="H27">
+        <v>13.78</v>
+      </c>
+      <c r="I27">
+        <v>0.48</v>
+      </c>
+      <c r="J27">
+        <v>25.19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" t="s">
+        <v>117</v>
+      </c>
+      <c r="D28" t="s">
+        <v>118</v>
+      </c>
+      <c r="E28" t="s">
+        <v>119</v>
+      </c>
+      <c r="F28" t="s">
+        <v>120</v>
+      </c>
+      <c r="G28" t="s">
+        <v>121</v>
+      </c>
+      <c r="H28" t="s">
+        <v>122</v>
+      </c>
+      <c r="I28" t="s">
+        <v>123</v>
+      </c>
+      <c r="J28" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29">
+        <v>0.36</v>
+      </c>
+      <c r="D29">
+        <v>0.22</v>
+      </c>
+      <c r="E29">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="F29">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="G29">
+        <v>0.44</v>
+      </c>
+      <c r="H29">
+        <v>1.04</v>
+      </c>
+      <c r="I29">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="J29">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30">
+        <v>0.08</v>
+      </c>
+      <c r="D30">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E30">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="F30">
+        <v>0.02</v>
+      </c>
+      <c r="G30">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="H30">
+        <v>0.23</v>
+      </c>
+      <c r="I30">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J30">
+        <v>0.42</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{64821D71-4ADF-478C-9F88-694549E7FE67}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C3B4E1F-9E03-4EDC-9D05-C2C567A5D179}">
+  <dimension ref="A1:F41"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="36.33203125" customWidth="1"/>
+    <col min="3" max="3" width="40.77734375" customWidth="1"/>
+    <col min="6" max="6" width="69" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C13" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>149</v>
+      </c>
+      <c r="C14" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>153</v>
+      </c>
+      <c r="C16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>155</v>
+      </c>
+      <c r="C17" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>158</v>
+      </c>
+      <c r="C19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>157</v>
+      </c>
+      <c r="C20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>161</v>
+      </c>
+      <c r="C21" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>163</v>
+      </c>
+      <c r="C22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>165</v>
+      </c>
+      <c r="C23" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>168</v>
+      </c>
+      <c r="C25" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>167</v>
+      </c>
+      <c r="C26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>171</v>
+      </c>
+      <c r="C27" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>175</v>
+      </c>
+      <c r="C29" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>25</v>
+      </c>
+      <c r="B31" t="s">
+        <v>178</v>
+      </c>
+      <c r="C31" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
+        <v>177</v>
+      </c>
+      <c r="C32" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>27</v>
+      </c>
+      <c r="B33" t="s">
+        <v>181</v>
+      </c>
+      <c r="C33" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>28</v>
+      </c>
+      <c r="B34" t="s">
+        <v>183</v>
+      </c>
+      <c r="C34" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>29</v>
+      </c>
+      <c r="B35" t="s">
+        <v>185</v>
+      </c>
+      <c r="C35" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>30</v>
+      </c>
+      <c r="B37" t="s">
+        <v>187</v>
+      </c>
+      <c r="C37" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>31</v>
+      </c>
+      <c r="B38" t="s">
+        <v>189</v>
+      </c>
+      <c r="C38" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>32</v>
+      </c>
+      <c r="B39" t="s">
+        <v>191</v>
+      </c>
+      <c r="C39" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>33</v>
+      </c>
+      <c r="B40" t="s">
+        <v>193</v>
+      </c>
+      <c r="C40" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>34</v>
+      </c>
+      <c r="B41" t="s">
+        <v>195</v>
+      </c>
+      <c r="C41" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{B44D4F50-0E09-49A8-864D-F6F860FEC704}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added more findings on geomorphological data
</commit_message>
<xml_diff>
--- a/uranium.xlsx
+++ b/uranium.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ikansh\CS\uranium-soil-analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ikansh\CS\uranium-punjab-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA730C9E-E9E8-4FB0-82B7-A323A9F1A70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AE6D12-7EB7-412E-B5DB-08F186363309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="High U-contents observed in som" sheetId="1" r:id="rId1"/>
     <sheet name="Uranium Content Anomalies in Gr" sheetId="2" r:id="rId2"/>
     <sheet name="Comparative statistical analysi" sheetId="3" r:id="rId3"/>
     <sheet name="Uranium studies in water sample" sheetId="4" r:id="rId4"/>
+    <sheet name="Elevated Uranium and Toxic Elem" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="200">
   <si>
     <t>Location</t>
   </si>
@@ -625,6 +626,9 @@
   </si>
   <si>
     <t>https://www.sciencedirect.com/science/article/pii/S1350448707000492</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s12403-014-0144-4</t>
   </si>
 </sst>
 </file>
@@ -632,8 +636,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="[$-14009]yyyy/mm/dd;@"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+    <numFmt numFmtId="164" formatCode="[$-14009]yyyy/mm/dd;@"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -683,12 +687,12 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -705,6 +709,235 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1027" name="AutoShape 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90D27403-C319-0D66-A977-F75C836DC54C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="548640"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF49C66F-5D85-E824-8D11-FE3CB4C6973E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="640080" y="548640"/>
+          <a:ext cx="5410200" cy="5162550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>34290</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34CC8CB6-E342-4C7C-D56C-2633A396092A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6667500" y="457200"/>
+          <a:ext cx="5410200" cy="5429250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>32385</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BACE3BC4-DF8D-C817-1A58-A0E8815126DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12793980" y="441960"/>
+          <a:ext cx="5715000" cy="5076825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>102870</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2ED4475F-4647-18B6-969F-09FD63D7EAC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18897600" y="434340"/>
+          <a:ext cx="6524625" cy="7715250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -972,7 +1205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -2836,7 +3069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C3B4E1F-9E03-4EDC-9D05-C2C567A5D179}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -3272,4 +3505,31 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62CEE51B-1925-49A4-BAC0-5B53941B4C97}">
+  <dimension ref="C35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="51" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C35" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C35" r:id="rId1" xr:uid="{3631D9F1-871B-4B8D-94E1-ACF9EEBDC6DD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>